<commit_message>
Auto-committed on 2023/09/26 週二 16:43:39.39
</commit_message>
<xml_diff>
--- a/Program/Other/LM074_底稿_B040金融機構承作｢公司法人購置住宅貸款｣統計表.xlsx
+++ b/Program/Other/LM074_底稿_B040金融機構承作｢公司法人購置住宅貸款｣統計表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57C1975-3EE9-46E2-A915-F6A0D7228E9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710E049C-DA38-41EC-A1DD-1E8C8C33ED22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B50B7979-97DD-44E6-B1C4-A6E1266EFB36}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{B50B7979-97DD-44E6-B1C4-A6E1266EFB36}"/>
   </bookViews>
   <sheets>
     <sheet name="FOA" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <r>
       <t>B040-</t>
@@ -101,10 +101,6 @@
       </rPr>
       <t>資料期間：</t>
     </r>
-  </si>
-  <si>
-    <t>民國    年    月</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>[位數檢核]</t>
@@ -1560,30 +1556,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679AA6AA-E9E5-4642-AD6A-549D32817E3E}">
   <dimension ref="A1:BK27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:F5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" customWidth="1"/>
-    <col min="9" max="9" width="15.77734375" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
-    <col min="11" max="11" width="30.33203125" customWidth="1"/>
-    <col min="13" max="20" width="8.44140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" customWidth="1"/>
+    <col min="6" max="6" width="16.90625" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" customWidth="1"/>
+    <col min="8" max="8" width="18.1796875" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" customWidth="1"/>
+    <col min="10" max="10" width="14.90625" customWidth="1"/>
+    <col min="11" max="11" width="30.36328125" customWidth="1"/>
+    <col min="13" max="20" width="8.453125" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
-    <col min="22" max="29" width="8.44140625" hidden="1" customWidth="1"/>
-    <col min="53" max="54" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="29" width="8.453125" hidden="1" customWidth="1"/>
+    <col min="53" max="54" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="58" max="60" width="6" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="2.6328125" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1647,19 +1643,19 @@
       <c r="AZ1" s="2"/>
       <c r="BA1" s="3" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(E3," ",""),"　","")</f>
-        <v>民國年月</v>
-      </c>
-      <c r="BB1" s="3" t="str">
+        <v/>
+      </c>
+      <c r="BB1" s="3" t="e">
         <f>LEFT(BA1,FIND("月",BA1,1))</f>
-        <v>民國年月</v>
-      </c>
-      <c r="BC1" s="4" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="BC1" s="4" t="e">
         <f>MID(BA1,FIND("民國",BA1,1)+2,FIND("年",BA1,1)-FIND("民國",BA1,1)-2)</f>
-        <v/>
-      </c>
-      <c r="BD1" s="4" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="BD1" s="4" t="e">
         <f>MID(BA1,FIND("年",BA1,1)+1,FIND("月",BA1,1)-FIND("年",BA1,1)-1)</f>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="BE1" s="4" t="e">
         <f>(BC1+1911) &amp; RIGHT("0" &amp; BD1,2)</f>
@@ -1756,9 +1752,7 @@
       <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="31" t="s">
-        <v>7</v>
-      </c>
+      <c r="E3" s="31"/>
       <c r="F3" s="31"/>
       <c r="G3" s="31"/>
       <c r="H3" s="2"/>
@@ -1818,7 +1812,7 @@
       <c r="BJ3" s="2"/>
       <c r="BK3" s="2"/>
     </row>
-    <row r="4" spans="1:63" ht="19.8">
+    <row r="4" spans="1:63" ht="19.5">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1832,7 +1826,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N4" s="32"/>
       <c r="O4" s="2"/>
@@ -1887,48 +1881,48 @@
     </row>
     <row r="5" spans="1:63">
       <c r="A5" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="C5" s="37" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>11</v>
       </c>
       <c r="D5" s="38"/>
       <c r="E5" s="38"/>
       <c r="F5" s="39"/>
       <c r="G5" s="40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="38"/>
       <c r="I5" s="38"/>
       <c r="J5" s="39"/>
       <c r="K5" s="41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N5" s="38"/>
       <c r="O5" s="38"/>
       <c r="P5" s="39"/>
       <c r="Q5" s="40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R5" s="38"/>
       <c r="S5" s="38"/>
       <c r="T5" s="39"/>
       <c r="U5" s="2"/>
       <c r="V5" s="37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W5" s="38"/>
       <c r="X5" s="38"/>
       <c r="Y5" s="39"/>
       <c r="Z5" s="40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AA5" s="38"/>
       <c r="AB5" s="38"/>
@@ -1968,83 +1962,83 @@
       <c r="BJ5" s="2"/>
       <c r="BK5" s="2"/>
     </row>
-    <row r="6" spans="1:63" ht="37.799999999999997">
+    <row r="6" spans="1:63" ht="37.5">
       <c r="A6" s="34"/>
       <c r="B6" s="36"/>
       <c r="C6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="F6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>17</v>
-      </c>
       <c r="G6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="J6" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="K6" s="41"/>
       <c r="L6" s="10"/>
       <c r="M6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="O6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="11" t="s">
-        <v>16</v>
-      </c>
       <c r="P6" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="R6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="S6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="S6" s="11" t="s">
-        <v>16</v>
-      </c>
       <c r="T6" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U6" s="10"/>
       <c r="V6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="W6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="W6" s="11" t="s">
+      <c r="X6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="X6" s="11" t="s">
-        <v>16</v>
-      </c>
       <c r="Y6" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Z6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="AA6" s="11" t="s">
+      <c r="AB6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AB6" s="11" t="s">
-        <v>16</v>
-      </c>
       <c r="AC6" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AD6" s="10"/>
       <c r="AE6" s="10"/>
@@ -2083,19 +2077,35 @@
     </row>
     <row r="7" spans="1:63" ht="30" customHeight="1">
       <c r="A7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
+      <c r="C7" s="27">
+        <v>0</v>
+      </c>
+      <c r="D7" s="28">
+        <v>0</v>
+      </c>
+      <c r="E7" s="28">
+        <v>0</v>
+      </c>
+      <c r="F7" s="28">
+        <v>0</v>
+      </c>
+      <c r="G7" s="27">
+        <v>0</v>
+      </c>
+      <c r="H7" s="28">
+        <v>0</v>
+      </c>
+      <c r="I7" s="28">
+        <v>0</v>
+      </c>
+      <c r="J7" s="28">
+        <v>0</v>
+      </c>
       <c r="K7" s="15" t="str">
         <f>M7&amp;N7&amp;O7&amp;P7&amp;Q7&amp;R7&amp;S7&amp;T7&amp;X7&amp;AB7</f>
         <v/>
@@ -2185,19 +2195,35 @@
     </row>
     <row r="8" spans="1:63" ht="30" customHeight="1">
       <c r="A8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
+      <c r="C8" s="27">
+        <v>0</v>
+      </c>
+      <c r="D8" s="28">
+        <v>0</v>
+      </c>
+      <c r="E8" s="28">
+        <v>0</v>
+      </c>
+      <c r="F8" s="28">
+        <v>0</v>
+      </c>
+      <c r="G8" s="27">
+        <v>0</v>
+      </c>
+      <c r="H8" s="28">
+        <v>0</v>
+      </c>
+      <c r="I8" s="28">
+        <v>0</v>
+      </c>
+      <c r="J8" s="28">
+        <v>0</v>
+      </c>
       <c r="K8" s="15" t="str">
         <f t="shared" ref="K8:K13" si="10">M8&amp;N8&amp;O8&amp;P8&amp;Q8&amp;R8&amp;S8&amp;T8&amp;X8&amp;AB8</f>
         <v/>
@@ -2287,19 +2313,35 @@
     </row>
     <row r="9" spans="1:63" ht="30" customHeight="1">
       <c r="A9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
+      <c r="C9" s="27">
+        <v>0</v>
+      </c>
+      <c r="D9" s="28">
+        <v>0</v>
+      </c>
+      <c r="E9" s="28">
+        <v>0</v>
+      </c>
+      <c r="F9" s="28">
+        <v>0</v>
+      </c>
+      <c r="G9" s="27">
+        <v>0</v>
+      </c>
+      <c r="H9" s="28">
+        <v>0</v>
+      </c>
+      <c r="I9" s="28">
+        <v>0</v>
+      </c>
+      <c r="J9" s="28">
+        <v>0</v>
+      </c>
       <c r="K9" s="15" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -2389,19 +2431,35 @@
     </row>
     <row r="10" spans="1:63" ht="30" customHeight="1">
       <c r="A10" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
+      <c r="C10" s="27">
+        <v>0</v>
+      </c>
+      <c r="D10" s="28">
+        <v>0</v>
+      </c>
+      <c r="E10" s="28">
+        <v>0</v>
+      </c>
+      <c r="F10" s="28">
+        <v>0</v>
+      </c>
+      <c r="G10" s="27">
+        <v>0</v>
+      </c>
+      <c r="H10" s="28">
+        <v>0</v>
+      </c>
+      <c r="I10" s="28">
+        <v>0</v>
+      </c>
+      <c r="J10" s="28">
+        <v>0</v>
+      </c>
       <c r="K10" s="15" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -2491,19 +2549,35 @@
     </row>
     <row r="11" spans="1:63" ht="30" customHeight="1">
       <c r="A11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
+      <c r="C11" s="27">
+        <v>0</v>
+      </c>
+      <c r="D11" s="28">
+        <v>0</v>
+      </c>
+      <c r="E11" s="28">
+        <v>0</v>
+      </c>
+      <c r="F11" s="28">
+        <v>0</v>
+      </c>
+      <c r="G11" s="27">
+        <v>0</v>
+      </c>
+      <c r="H11" s="28">
+        <v>0</v>
+      </c>
+      <c r="I11" s="28">
+        <v>0</v>
+      </c>
+      <c r="J11" s="28">
+        <v>0</v>
+      </c>
       <c r="K11" s="15" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -2593,19 +2667,35 @@
     </row>
     <row r="12" spans="1:63" ht="30" customHeight="1">
       <c r="A12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
+      <c r="C12" s="27">
+        <v>0</v>
+      </c>
+      <c r="D12" s="28">
+        <v>0</v>
+      </c>
+      <c r="E12" s="28">
+        <v>0</v>
+      </c>
+      <c r="F12" s="28">
+        <v>0</v>
+      </c>
+      <c r="G12" s="27">
+        <v>0</v>
+      </c>
+      <c r="H12" s="28">
+        <v>0</v>
+      </c>
+      <c r="I12" s="28">
+        <v>0</v>
+      </c>
+      <c r="J12" s="28">
+        <v>0</v>
+      </c>
       <c r="K12" s="15" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -2695,19 +2785,35 @@
     </row>
     <row r="13" spans="1:63" ht="30" customHeight="1">
       <c r="A13" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
+      <c r="C13" s="27">
+        <v>0</v>
+      </c>
+      <c r="D13" s="28">
+        <v>0</v>
+      </c>
+      <c r="E13" s="28">
+        <v>0</v>
+      </c>
+      <c r="F13" s="28">
+        <v>0</v>
+      </c>
+      <c r="G13" s="27">
+        <v>0</v>
+      </c>
+      <c r="H13" s="28">
+        <v>0</v>
+      </c>
+      <c r="I13" s="28">
+        <v>0</v>
+      </c>
+      <c r="J13" s="28">
+        <v>0</v>
+      </c>
       <c r="K13" s="15" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -2797,10 +2903,10 @@
     </row>
     <row r="14" spans="1:63" ht="30" customHeight="1">
       <c r="A14" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>33</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>34</v>
       </c>
       <c r="C14" s="20">
         <f>SUM(C7:C13)</f>
@@ -2941,7 +3047,7 @@
     </row>
     <row r="15" spans="1:63">
       <c r="A15" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="42"/>
       <c r="C15" s="42"/>
@@ -3008,18 +3114,18 @@
     </row>
     <row r="16" spans="1:63" ht="30" customHeight="1">
       <c r="A16" s="43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="44"/>
       <c r="C16" s="45"/>
       <c r="D16" s="46"/>
       <c r="E16" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F16" s="45"/>
       <c r="G16" s="46"/>
       <c r="H16" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I16" s="45"/>
       <c r="J16" s="46"/>
@@ -3079,18 +3185,18 @@
     </row>
     <row r="17" spans="1:63" ht="30" customHeight="1">
       <c r="A17" s="43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="44"/>
       <c r="C17" s="45"/>
       <c r="D17" s="46"/>
       <c r="E17" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" s="45"/>
       <c r="G17" s="46"/>
       <c r="H17" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I17" s="45"/>
       <c r="J17" s="46"/>
@@ -3150,18 +3256,18 @@
     </row>
     <row r="18" spans="1:63" ht="30" customHeight="1">
       <c r="A18" s="43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="44"/>
       <c r="C18" s="47"/>
       <c r="D18" s="46"/>
       <c r="E18" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="45"/>
       <c r="G18" s="46"/>
       <c r="H18" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I18" s="45"/>
       <c r="J18" s="46"/>
@@ -3286,7 +3392,7 @@
     </row>
     <row r="20" spans="1:63">
       <c r="A20" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -3353,7 +3459,7 @@
     </row>
     <row r="21" spans="1:63">
       <c r="A21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3420,7 +3526,7 @@
     </row>
     <row r="22" spans="1:63">
       <c r="A22" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3487,7 +3593,7 @@
     </row>
     <row r="23" spans="1:63">
       <c r="A23" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -3554,7 +3660,7 @@
     </row>
     <row r="24" spans="1:63">
       <c r="A24" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3621,7 +3727,7 @@
     </row>
     <row r="25" spans="1:63">
       <c r="A25" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3688,7 +3794,7 @@
     </row>
     <row r="26" spans="1:63">
       <c r="A26" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -3755,7 +3861,7 @@
     </row>
     <row r="27" spans="1:63">
       <c r="A27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>

</xml_diff>